<commit_message>
task modified and completed
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/task1.xlsx
+++ b/src/test/resources/excel/task1.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="1">
   <si>
-    <t>APPLE iPhone SE (Black, 64 GB)</t>
+    <t>APPLE iPhone SE (White, 128 GB)</t>
   </si>
 </sst>
 </file>
@@ -71,152 +71,152 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="C3" t="s">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="D4" t="s">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="E5" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="F6" t="s">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="G7" t="s">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="H8" t="s">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="I9" t="s">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="J10" t="s">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="K11" t="s">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="L12" t="s">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="M13" t="s">
+      <c r="A13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="N14" t="s">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="O15" t="s">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="P16" t="s">
+      <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="Q17" t="s">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="R18" t="s">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="S19" t="s">
+      <c r="A19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="T20" t="s">
+      <c r="A20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21">
-      <c r="U21" t="s">
+      <c r="A21" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22">
-      <c r="V22" t="s">
+      <c r="A22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="W23" t="s">
+      <c r="A23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="X24" t="s">
+      <c r="A24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="Y25" t="s">
+      <c r="A25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="Z26" t="s">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="AA27" t="s">
+      <c r="A27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="AB28" t="s">
+      <c r="A28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="AC29" t="s">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="AD30" t="s">
+      <c r="A30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="AE31" t="s">
+      <c r="A31" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>